<commit_message>
- Connect the VCCIO pin of the FTDI IC to the 3.3V - Improve the layout to offer better thermal conductivity for the LDO
</commit_message>
<xml_diff>
--- a/Rleased/BOM/USB_FTDI.xlsx
+++ b/Rleased/BOM/USB_FTDI.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Projects\FTDI\USB-FTDI\USB-FTDI\Rleased\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Projects\USB-FTDI\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A599F6D8-1666-463E-927C-04BB2FFD8BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0343FE-74D8-48EF-8025-A654A5335C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H16R6" sheetId="1" r:id="rId1"/>
+    <sheet name="USB_FTDI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Hexabitz Kits</t>
   </si>
   <si>
-    <t>USB-FTDI</t>
-  </si>
-  <si>
     <t>C3225X5R0J107M250AC</t>
   </si>
   <si>
@@ -134,12 +131,6 @@
     <t>CAP CERAMIC TOR 100UF 6.3V X5R 20% 1210</t>
   </si>
   <si>
-    <t>CAP CER 0.1uF 10% x7R 0603 10V</t>
-  </si>
-  <si>
-    <t>C0603C104K8RACTU</t>
-  </si>
-  <si>
     <t>https://octopart.com/c0603c103k5ractu-kemet-133094?r=sp&amp;s=R_iPBxLnSmGqhkU2rIMFpg</t>
   </si>
   <si>
@@ -158,15 +149,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>CAP TANT 1UF 16V 20% 0805</t>
-  </si>
-  <si>
-    <t>TAJR105M016RNG</t>
-  </si>
-  <si>
-    <t>AVX</t>
-  </si>
-  <si>
     <t>Multilayer Ceramic Capacitor, 47 pF, 50 V, ± 5%, C0G (NP0), 0603 [1608 Metric]</t>
   </si>
   <si>
@@ -227,15 +209,6 @@
     <t>https://octopart.com/vlmo1300-gs08-vishay-21709200?r=sp#</t>
   </si>
   <si>
-    <t>4.7uF Solid Polymer Tantalum Capacitor; 10 V dc +/-20%; POSCAP Series</t>
-  </si>
-  <si>
-    <t>10TPU4R7MSI</t>
-  </si>
-  <si>
-    <t>https://octopart.com/10tpu4r7msi-panasonic-29487748</t>
-  </si>
-  <si>
     <t>FT232RL-REEL</t>
   </si>
   <si>
@@ -263,9 +236,6 @@
     <t>4 Position 30 VAC 3 A USB Type A 2.0 Right Angle Receptacle USB Connector</t>
   </si>
   <si>
-    <t>https://octopart.com/tajr105m016rnj-avx-1188552?r=sp</t>
-  </si>
-  <si>
     <t>FTDI</t>
   </si>
   <si>
@@ -279,6 +249,42 @@
   </si>
   <si>
     <t>C6, C7 , C9, C10</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>C0805C475K4RACTU</t>
+  </si>
+  <si>
+    <t>KEMET [VA]</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0805c475k4ractu-kemet-22859922?r=sp</t>
+  </si>
+  <si>
+    <t>CAP CER 1 UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>CC0805KKX7R7BB105</t>
+  </si>
+  <si>
+    <t>YAGEO [VA]</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>CGA3E2X8R1E104K080AE</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cga3e2x8r1e104k080ae-tdk-68305753?r=sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB to FTDI with 3.3V/1A </t>
   </si>
 </sst>
 </file>
@@ -925,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -987,7 +993,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -1004,7 +1010,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="21">
-        <v>45332</v>
+        <v>45535</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="23"/>
@@ -1015,7 +1021,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1047,19 +1053,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F9" s="18">
         <v>1</v>
@@ -1067,19 +1073,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="18">
         <v>1</v>
@@ -1087,19 +1093,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="F11" s="18">
         <v>4</v>
@@ -1107,19 +1113,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F12" s="18">
         <v>2</v>
@@ -1130,16 +1136,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F13" s="18">
         <v>1</v>
@@ -1147,19 +1153,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F14" s="18">
         <v>1</v>
@@ -1167,19 +1173,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>31</v>
-      </c>
       <c r="C15" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="18">
         <v>1</v>
@@ -1187,19 +1193,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F16" s="18">
         <v>2</v>
@@ -1207,19 +1213,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F17" s="18">
         <v>2</v>
@@ -1247,19 +1253,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F19" s="18">
         <v>1</v>
@@ -1267,19 +1273,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F20" s="18">
         <v>1</v>
@@ -1287,19 +1293,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="F21" s="18">
         <v>1</v>
@@ -1310,16 +1316,16 @@
         <v>18</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
@@ -1332,14 +1338,14 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{AEA5A507-67BA-49A5-88AE-1355C8B23939}"/>
-    <hyperlink ref="E18" r:id="rId2" xr:uid="{CC341C9A-DFE5-4F19-A8E0-FFB08B066D0D}"/>
-    <hyperlink ref="E16" r:id="rId3" xr:uid="{44C12A52-2C98-4020-89BC-EAFAD6C3C488}"/>
-    <hyperlink ref="E17" r:id="rId4" xr:uid="{A7CD2E14-7C67-4692-B467-99CAFCC96F3F}"/>
-    <hyperlink ref="E20" r:id="rId5" xr:uid="{1FB79B5E-8E80-4D81-8A1B-4976E895A80A}"/>
-    <hyperlink ref="E19" r:id="rId6" xr:uid="{F23127BD-79B1-4967-BE92-680CFE2FF599}"/>
-    <hyperlink ref="E14" r:id="rId7" xr:uid="{DC857922-F4B0-4F9E-AFFB-BA46A34B2EA4}"/>
-    <hyperlink ref="E22" r:id="rId8" xr:uid="{CB969912-49E7-4D8C-BE16-F45EB68AEDCF}"/>
+    <hyperlink ref="E18" r:id="rId1" xr:uid="{CC341C9A-DFE5-4F19-A8E0-FFB08B066D0D}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{44C12A52-2C98-4020-89BC-EAFAD6C3C488}"/>
+    <hyperlink ref="E17" r:id="rId3" xr:uid="{A7CD2E14-7C67-4692-B467-99CAFCC96F3F}"/>
+    <hyperlink ref="E20" r:id="rId4" xr:uid="{1FB79B5E-8E80-4D81-8A1B-4976E895A80A}"/>
+    <hyperlink ref="E19" r:id="rId5" xr:uid="{F23127BD-79B1-4967-BE92-680CFE2FF599}"/>
+    <hyperlink ref="E22" r:id="rId6" xr:uid="{CB969912-49E7-4D8C-BE16-F45EB68AEDCF}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{683A5FA8-3399-4D62-883B-1BE8D5FBA580}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{EAC5EC70-F2B3-4C02-9E22-8AE473EDFED0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>

</xml_diff>